<commit_message>
final commit before collabrate
</commit_message>
<xml_diff>
--- a/app/accounting/309000AG/PCE INV 402026.xlsx
+++ b/app/accounting/309000AG/PCE INV 402026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\00-Bridge Database\309000AG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A28FDB-6E39-46C2-90AF-1F5EAC645E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A784848-38DD-4384-8C2E-151CC2FE98AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5265" yWindow="2775" windowWidth="27075" windowHeight="11775" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
+    <workbookView xWindow="16080" yWindow="3360" windowWidth="29040" windowHeight="15720" xr2:uid="{9F1EA209-DB64-4862-B5BC-AB2E13480384}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="13" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Date:</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Car Park Ventilation CFD -Final Documentation</t>
+  </si>
+  <si>
+    <t>Variation</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="45">
-        <v>45334</v>
+        <v>45368</v>
       </c>
       <c r="K4" s="43"/>
       <c r="L4" s="7"/>
@@ -1350,7 +1353,9 @@
       <c r="U24" s="17"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
+      <c r="A25" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="F25" s="52"/>
       <c r="G25" s="53"/>
       <c r="H25" s="48"/>

</xml_diff>